<commit_message>
#4 Implement in main
#4 Performance Fix - Finished
</commit_message>
<xml_diff>
--- a/others/materialenliste_Team-C_v2_01-03-2023.xlsx
+++ b/others/materialenliste_Team-C_v2_01-03-2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Gewachshaus\others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D7DCD3-6F9E-4714-869E-2E5E75FF07AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAC9D31-329E-4B46-8D75-2AD4731AC2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1089,9 +1089,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
@@ -1881,9 +1884,9 @@
     <hyperlink ref="D17" r:id="rId26" display="https://www.az-delivery.de/collections/leds/products/4-x-64er-led-matrix-display" xr:uid="{42A2BA48-4F70-4EB2-83AE-3039EF147617}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="57" orientation="portrait" r:id="rId27"/>
+  <pageSetup paperSize="9" scale="85" orientation="landscape" r:id="rId27"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;T&amp;C&amp;F&amp;R&amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;P&amp;C&amp;F&amp;R&amp;D</oddHeader>
   </headerFooter>
   <drawing r:id="rId28"/>
   <tableParts count="1">
@@ -1893,67 +1896,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FolderType xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <Owner xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Teachers xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <AppVersion xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <LMS_Mappings xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <Math_Settings xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <NotebookType xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <Students xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Templates xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <TeamsChannelId xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <Student_Groups xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Invited_Teachers xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <CultureName xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <Distribution_Groups xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <Invited_Students xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010017050FBCF721D74EA191A2597D5F1D5E" ma:contentTypeVersion="34" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0862e470fa0c0095e2669c6e4a75f78a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cfd14483-b7c0-45b9-993d-9132a74e282d" xmlns:ns4="ff8d2f56-c84d-4871-b762-e5ed0407f39a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b183421cabab6f235163586efe9e3efe" ns3:_="" ns4:_="">
     <xsd:import namespace="cfd14483-b7c0-45b9-993d-9132a74e282d"/>
@@ -2370,32 +2312,68 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CD87B84-825B-439A-B230-2787E5696C25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="ff8d2f56-c84d-4871-b762-e5ed0407f39a"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="cfd14483-b7c0-45b9-993d-9132a74e282d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547B504B-5F24-4A1D-A49E-39A88668BD81}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FolderType xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <Owner xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Teachers xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <AppVersion xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <LMS_Mappings xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <Math_Settings xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <NotebookType xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <Students xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Templates xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <TeamsChannelId xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <Student_Groups xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Invited_Teachers xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <CultureName xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <Distribution_Groups xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <Invited_Students xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="cfd14483-b7c0-45b9-993d-9132a74e282d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30E27BE0-1DF6-4FBB-BB95-A839F5DAD638}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2412,4 +2390,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547B504B-5F24-4A1D-A49E-39A88668BD81}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CD87B84-825B-439A-B230-2787E5696C25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="ff8d2f56-c84d-4871-b762-e5ed0407f39a"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="cfd14483-b7c0-45b9-993d-9132a74e282d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>